<commit_message>
update taxa column description
</commit_message>
<xml_diff>
--- a/TBN_VertebrateList_Big5/protected_species_list_TBN.xlsx
+++ b/TBN_VertebrateList_Big5/protected_species_list_TBN.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\物種名錄\保育類野生動物名錄\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="欄位說明" sheetId="2" r:id="rId1"/>
     <sheet name="保育類野生動物名錄(TBN)" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'保育類野生動物名錄(TBN)'!$A$1:$K$253</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'保育類野生動物名錄(TBN)'!$A$1:$M$253</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -2321,10 +2321,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>rank</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TBN學名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2345,10 +2341,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>分類階層</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>保育等級版本</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2381,9 +2373,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>species</t>
-  </si>
-  <si>
     <t xml:space="preserve">Scientific name_TBN </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2416,13 +2405,25 @@
   </si>
   <si>
     <t>Version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rank_PSL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>林務局保育類名錄使用學名的分類階層</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rank_PSL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2944,20 +2945,21 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="B1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2965,7 +2967,7 @@
         <v>745</v>
       </c>
       <c r="B2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2973,36 +2975,36 @@
         <v>744</v>
       </c>
       <c r="B3" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="B4" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="B5" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="B6" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -3010,42 +3012,42 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="B8" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="B9" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>746</v>
+        <v>768</v>
       </c>
       <c r="B10" t="s">
-        <v>752</v>
+        <v>769</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B12" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B13" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
   </sheetData>
@@ -3060,13 +3062,13 @@
   <dimension ref="A1:M253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.375" customWidth="1"/>
+    <col min="1" max="1" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.25" customWidth="1"/>
@@ -3086,10 +3088,10 @@
         <v>744</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>0</v>
@@ -3104,7 +3106,7 @@
         <v>704</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>746</v>
+        <v>770</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3121,7 +3123,7 @@
         <v>508</v>
       </c>
       <c r="E2" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F2">
         <v>416105</v>
@@ -3153,7 +3155,7 @@
         <v>509</v>
       </c>
       <c r="E3" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F3">
         <v>1024882</v>
@@ -3183,7 +3185,7 @@
         <v>508</v>
       </c>
       <c r="E4" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F4">
         <v>1024484</v>
@@ -3213,7 +3215,7 @@
         <v>509</v>
       </c>
       <c r="E5" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F5">
         <v>1024697</v>
@@ -3243,7 +3245,7 @@
         <v>508</v>
       </c>
       <c r="E6" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F6">
         <v>1024735</v>
@@ -3273,7 +3275,7 @@
         <v>509</v>
       </c>
       <c r="E7" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F7">
         <v>1025759</v>
@@ -3303,7 +3305,7 @@
         <v>507</v>
       </c>
       <c r="E8" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F8">
         <v>1025768</v>
@@ -3333,7 +3335,7 @@
         <v>507</v>
       </c>
       <c r="E9" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F9">
         <v>1023992</v>
@@ -3363,7 +3365,7 @@
         <v>507</v>
       </c>
       <c r="E10" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F10" s="1">
         <v>1024731</v>
@@ -3375,8 +3377,8 @@
       <c r="I10">
         <v>188</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>761</v>
+      <c r="J10" t="s">
+        <v>726</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -3395,7 +3397,7 @@
         <v>507</v>
       </c>
       <c r="E11" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F11">
         <v>380580</v>
@@ -3427,7 +3429,7 @@
         <v>507</v>
       </c>
       <c r="E12" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F12">
         <v>380056</v>
@@ -3459,7 +3461,7 @@
         <v>507</v>
       </c>
       <c r="E13" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F13">
         <v>380062</v>
@@ -3491,7 +3493,7 @@
         <v>507</v>
       </c>
       <c r="E14" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F14">
         <v>380074</v>
@@ -3523,7 +3525,7 @@
         <v>508</v>
       </c>
       <c r="E15" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F15">
         <v>380162</v>
@@ -3555,7 +3557,7 @@
         <v>507</v>
       </c>
       <c r="E16" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F16">
         <v>380163</v>
@@ -3587,7 +3589,7 @@
         <v>507</v>
       </c>
       <c r="E17" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F17">
         <v>420867</v>
@@ -3619,7 +3621,7 @@
         <v>508</v>
       </c>
       <c r="E18" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F18">
         <v>1023790</v>
@@ -3649,7 +3651,7 @@
         <v>508</v>
       </c>
       <c r="E19" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F19">
         <v>1024659</v>
@@ -3679,7 +3681,7 @@
         <v>508</v>
       </c>
       <c r="E20" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F20">
         <v>380230</v>
@@ -3711,7 +3713,7 @@
         <v>508</v>
       </c>
       <c r="E21" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F21">
         <v>1024943</v>
@@ -3741,7 +3743,7 @@
         <v>508</v>
       </c>
       <c r="E22" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F22">
         <v>380236</v>
@@ -3773,7 +3775,7 @@
         <v>509</v>
       </c>
       <c r="E23" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F23">
         <v>380248</v>
@@ -3805,7 +3807,7 @@
         <v>508</v>
       </c>
       <c r="E24" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F24">
         <v>380222</v>
@@ -3837,7 +3839,7 @@
         <v>508</v>
       </c>
       <c r="E25" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F25">
         <v>1025729</v>
@@ -3867,7 +3869,7 @@
         <v>507</v>
       </c>
       <c r="E26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F26">
         <v>380128</v>
@@ -3899,7 +3901,7 @@
         <v>508</v>
       </c>
       <c r="E27" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F27">
         <v>380132</v>
@@ -3931,7 +3933,7 @@
         <v>509</v>
       </c>
       <c r="E28" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F28">
         <v>404565</v>
@@ -3963,7 +3965,7 @@
         <v>507</v>
       </c>
       <c r="E29" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F29">
         <v>380153</v>
@@ -3995,7 +3997,7 @@
         <v>509</v>
       </c>
       <c r="E30" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F30">
         <v>380257</v>
@@ -4027,7 +4029,7 @@
         <v>507</v>
       </c>
       <c r="E31" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F31">
         <v>1025242</v>
@@ -4057,7 +4059,7 @@
         <v>509</v>
       </c>
       <c r="E32" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F32">
         <v>380259</v>
@@ -4089,7 +4091,7 @@
         <v>507</v>
       </c>
       <c r="E33" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F33">
         <v>380260</v>
@@ -4121,7 +4123,7 @@
         <v>507</v>
       </c>
       <c r="E34" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F34">
         <v>1025693</v>
@@ -4151,7 +4153,7 @@
         <v>508</v>
       </c>
       <c r="E35" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F35">
         <v>1024716</v>
@@ -4181,7 +4183,7 @@
         <v>507</v>
       </c>
       <c r="E36" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F36">
         <v>1023423</v>
@@ -4211,7 +4213,7 @@
         <v>507</v>
       </c>
       <c r="E37" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F37">
         <v>1023424</v>
@@ -4241,7 +4243,7 @@
         <v>507</v>
       </c>
       <c r="E38" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F38">
         <v>380099</v>
@@ -4273,7 +4275,7 @@
         <v>507</v>
       </c>
       <c r="E39" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F39">
         <v>1023425</v>
@@ -4303,7 +4305,7 @@
         <v>507</v>
       </c>
       <c r="E40" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F40">
         <v>1023426</v>
@@ -4333,7 +4335,7 @@
         <v>507</v>
       </c>
       <c r="E41" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F41">
         <v>380105</v>
@@ -4365,7 +4367,7 @@
         <v>507</v>
       </c>
       <c r="E42" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F42">
         <v>1023965</v>
@@ -4395,7 +4397,7 @@
         <v>507</v>
       </c>
       <c r="E43" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F43">
         <v>380109</v>
@@ -4427,7 +4429,7 @@
         <v>507</v>
       </c>
       <c r="E44" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F44">
         <v>1023966</v>
@@ -4457,7 +4459,7 @@
         <v>507</v>
       </c>
       <c r="E45" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F45">
         <v>1024209</v>
@@ -4487,7 +4489,7 @@
         <v>509</v>
       </c>
       <c r="E46" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F46">
         <v>421135</v>
@@ -4519,7 +4521,7 @@
         <v>507</v>
       </c>
       <c r="E47" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F47">
         <v>1024812</v>
@@ -4549,7 +4551,7 @@
         <v>507</v>
       </c>
       <c r="E48" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F48">
         <v>1025068</v>
@@ -4579,7 +4581,7 @@
         <v>507</v>
       </c>
       <c r="E49" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F49">
         <v>1025168</v>
@@ -4609,7 +4611,7 @@
         <v>507</v>
       </c>
       <c r="E50" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F50">
         <v>1025516</v>
@@ -4639,7 +4641,7 @@
         <v>509</v>
       </c>
       <c r="E51" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F51">
         <v>1024929</v>
@@ -4669,7 +4671,7 @@
         <v>507</v>
       </c>
       <c r="E52" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F52">
         <v>1024354</v>
@@ -4699,7 +4701,7 @@
         <v>507</v>
       </c>
       <c r="E53" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F53">
         <v>1024355</v>
@@ -4729,7 +4731,7 @@
         <v>507</v>
       </c>
       <c r="E54" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F54">
         <v>1024356</v>
@@ -4759,7 +4761,7 @@
         <v>508</v>
       </c>
       <c r="E55" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F55">
         <v>380285</v>
@@ -4791,7 +4793,7 @@
         <v>507</v>
       </c>
       <c r="E56" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F56">
         <v>380289</v>
@@ -4823,7 +4825,7 @@
         <v>507</v>
       </c>
       <c r="E57" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F57">
         <v>1025193</v>
@@ -4853,7 +4855,7 @@
         <v>509</v>
       </c>
       <c r="E58" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F58">
         <v>380293</v>
@@ -4885,7 +4887,7 @@
         <v>509</v>
       </c>
       <c r="E59" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F59">
         <v>380294</v>
@@ -4917,7 +4919,7 @@
         <v>508</v>
       </c>
       <c r="E60" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F60">
         <v>380298</v>
@@ -4949,7 +4951,7 @@
         <v>507</v>
       </c>
       <c r="E61" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F61">
         <v>1024015</v>
@@ -4979,7 +4981,7 @@
         <v>508</v>
       </c>
       <c r="E62" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F62">
         <v>380336</v>
@@ -5011,7 +5013,7 @@
         <v>507</v>
       </c>
       <c r="E63" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F63">
         <v>404581</v>
@@ -5043,7 +5045,7 @@
         <v>507</v>
       </c>
       <c r="E64" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F64">
         <v>1024219</v>
@@ -5073,7 +5075,7 @@
         <v>508</v>
       </c>
       <c r="E65" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F65">
         <v>1024676</v>
@@ -5103,7 +5105,7 @@
         <v>508</v>
       </c>
       <c r="E66" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F66">
         <v>425192</v>
@@ -5135,7 +5137,7 @@
         <v>508</v>
       </c>
       <c r="E67" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F67">
         <v>1025318</v>
@@ -5165,7 +5167,7 @@
         <v>508</v>
       </c>
       <c r="E68" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F68">
         <v>1024598</v>
@@ -5195,7 +5197,7 @@
         <v>508</v>
       </c>
       <c r="E69" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F69">
         <v>380455</v>
@@ -5227,7 +5229,7 @@
         <v>507</v>
       </c>
       <c r="E70" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F70">
         <v>1024395</v>
@@ -5257,7 +5259,7 @@
         <v>507</v>
       </c>
       <c r="E71" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F71">
         <v>404589</v>
@@ -5289,7 +5291,7 @@
         <v>507</v>
       </c>
       <c r="E72" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F72">
         <v>428597</v>
@@ -5321,7 +5323,7 @@
         <v>507</v>
       </c>
       <c r="E73" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F73">
         <v>428595</v>
@@ -5353,7 +5355,7 @@
         <v>508</v>
       </c>
       <c r="E74" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F74">
         <v>380468</v>
@@ -5385,7 +5387,7 @@
         <v>508</v>
       </c>
       <c r="E75" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F75">
         <v>380467</v>
@@ -5417,7 +5419,7 @@
         <v>507</v>
       </c>
       <c r="E76" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F76">
         <v>1025642</v>
@@ -5447,7 +5449,7 @@
         <v>507</v>
       </c>
       <c r="E77" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F77">
         <v>1024234</v>
@@ -5477,7 +5479,7 @@
         <v>508</v>
       </c>
       <c r="E78" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F78">
         <v>1024921</v>
@@ -5507,7 +5509,7 @@
         <v>508</v>
       </c>
       <c r="E79" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F79">
         <v>1025204</v>
@@ -5537,7 +5539,7 @@
         <v>508</v>
       </c>
       <c r="E80" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F80">
         <v>1025629</v>
@@ -5567,7 +5569,7 @@
         <v>508</v>
       </c>
       <c r="E81" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F81">
         <v>419684</v>
@@ -5599,7 +5601,7 @@
         <v>507</v>
       </c>
       <c r="E82" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F82">
         <v>1025011</v>
@@ -5629,7 +5631,7 @@
         <v>507</v>
       </c>
       <c r="E83" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F83">
         <v>1025012</v>
@@ -5659,7 +5661,7 @@
         <v>508</v>
       </c>
       <c r="E84" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F84">
         <v>1025134</v>
@@ -5689,7 +5691,7 @@
         <v>508</v>
       </c>
       <c r="E85" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F85">
         <v>1025162</v>
@@ -5719,7 +5721,7 @@
         <v>507</v>
       </c>
       <c r="E86" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F86">
         <v>432166</v>
@@ -5751,7 +5753,7 @@
         <v>511</v>
       </c>
       <c r="E87" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F87">
         <v>1025140</v>
@@ -5781,7 +5783,7 @@
         <v>507</v>
       </c>
       <c r="E88" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F88">
         <v>380436</v>
@@ -5813,7 +5815,7 @@
         <v>507</v>
       </c>
       <c r="E89" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F89">
         <v>380440</v>
@@ -5845,7 +5847,7 @@
         <v>508</v>
       </c>
       <c r="E90" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F90">
         <v>380442</v>
@@ -5877,7 +5879,7 @@
         <v>507</v>
       </c>
       <c r="E91" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F91">
         <v>1023443</v>
@@ -5907,7 +5909,7 @@
         <v>507</v>
       </c>
       <c r="E92" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F92">
         <v>419446</v>
@@ -5939,7 +5941,7 @@
         <v>508</v>
       </c>
       <c r="E93" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F93">
         <v>404634</v>
@@ -5971,7 +5973,7 @@
         <v>507</v>
       </c>
       <c r="E94" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F94">
         <v>432360</v>
@@ -6003,7 +6005,7 @@
         <v>507</v>
       </c>
       <c r="E95" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F95">
         <v>417886</v>
@@ -6035,7 +6037,7 @@
         <v>507</v>
       </c>
       <c r="E96" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F96">
         <v>1025725</v>
@@ -6065,7 +6067,7 @@
         <v>508</v>
       </c>
       <c r="E97" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F97">
         <v>380486</v>
@@ -6097,7 +6099,7 @@
         <v>507</v>
       </c>
       <c r="E98" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F98">
         <v>1024117</v>
@@ -6127,7 +6129,7 @@
         <v>507</v>
       </c>
       <c r="E99" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F99">
         <v>1025227</v>
@@ -6157,7 +6159,7 @@
         <v>507</v>
       </c>
       <c r="E100" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F100">
         <v>419413</v>
@@ -6189,7 +6191,7 @@
         <v>507</v>
       </c>
       <c r="E101" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F101">
         <v>419414</v>
@@ -6221,7 +6223,7 @@
         <v>509</v>
       </c>
       <c r="E102" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F102">
         <v>419415</v>
@@ -6253,7 +6255,7 @@
         <v>509</v>
       </c>
       <c r="E103" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F103">
         <v>419416</v>
@@ -6285,7 +6287,7 @@
         <v>507</v>
       </c>
       <c r="E104" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F104">
         <v>417958</v>
@@ -6317,7 +6319,7 @@
         <v>509</v>
       </c>
       <c r="E105" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F105">
         <v>417808</v>
@@ -6349,7 +6351,7 @@
         <v>507</v>
       </c>
       <c r="E106" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F106">
         <v>1023655</v>
@@ -6379,7 +6381,7 @@
         <v>507</v>
       </c>
       <c r="E107" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F107">
         <v>1023656</v>
@@ -6409,7 +6411,7 @@
         <v>507</v>
       </c>
       <c r="E108" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F108">
         <v>1024414</v>
@@ -6439,7 +6441,7 @@
         <v>507</v>
       </c>
       <c r="E109" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F109">
         <v>380500</v>
@@ -6471,7 +6473,7 @@
         <v>507</v>
       </c>
       <c r="E110" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F110">
         <v>1024923</v>
@@ -6501,7 +6503,7 @@
         <v>507</v>
       </c>
       <c r="E111" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F111">
         <v>1025028</v>
@@ -6531,7 +6533,7 @@
         <v>507</v>
       </c>
       <c r="E112" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F112">
         <v>1025029</v>
@@ -6561,7 +6563,7 @@
         <v>507</v>
       </c>
       <c r="E113" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F113">
         <v>1025030</v>
@@ -6591,7 +6593,7 @@
         <v>507</v>
       </c>
       <c r="E114" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F114">
         <v>1025563</v>
@@ -6621,7 +6623,7 @@
         <v>507</v>
       </c>
       <c r="E115" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F115">
         <v>1025564</v>
@@ -6651,7 +6653,7 @@
         <v>509</v>
       </c>
       <c r="E116" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F116">
         <v>1025744</v>
@@ -6681,7 +6683,7 @@
         <v>507</v>
       </c>
       <c r="E117" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F117">
         <v>380622</v>
@@ -6713,7 +6715,7 @@
         <v>507</v>
       </c>
       <c r="E118" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F118">
         <v>380623</v>
@@ -6745,7 +6747,7 @@
         <v>507</v>
       </c>
       <c r="E119" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F119">
         <v>380627</v>
@@ -6777,7 +6779,7 @@
         <v>507</v>
       </c>
       <c r="E120" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F120">
         <v>380667</v>
@@ -6809,7 +6811,7 @@
         <v>507</v>
       </c>
       <c r="E121" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F121">
         <v>380674</v>
@@ -6841,7 +6843,7 @@
         <v>508</v>
       </c>
       <c r="E122" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F122">
         <v>380686</v>
@@ -6873,7 +6875,7 @@
         <v>509</v>
       </c>
       <c r="E123" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F123">
         <v>380630</v>
@@ -6905,7 +6907,7 @@
         <v>508</v>
       </c>
       <c r="E124" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F124">
         <v>427266</v>
@@ -6937,7 +6939,7 @@
         <v>510</v>
       </c>
       <c r="E125" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F125">
         <v>380642</v>
@@ -6969,7 +6971,7 @@
         <v>508</v>
       </c>
       <c r="E126" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F126">
         <v>380654</v>
@@ -7001,7 +7003,7 @@
         <v>507</v>
       </c>
       <c r="E127" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F127">
         <v>380657</v>
@@ -7033,7 +7035,7 @@
         <v>508</v>
       </c>
       <c r="E128" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F128">
         <v>380659</v>
@@ -7065,7 +7067,7 @@
         <v>507</v>
       </c>
       <c r="E129" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F129">
         <v>421733</v>
@@ -7097,7 +7099,7 @@
         <v>508</v>
       </c>
       <c r="E130" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F130">
         <v>1025481</v>
@@ -7127,7 +7129,7 @@
         <v>507</v>
       </c>
       <c r="E131" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F131">
         <v>421735</v>
@@ -7159,7 +7161,7 @@
         <v>507</v>
       </c>
       <c r="E132" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F132">
         <v>418194</v>
@@ -7191,7 +7193,7 @@
         <v>507</v>
       </c>
       <c r="E133" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F133">
         <v>427241</v>
@@ -7223,7 +7225,7 @@
         <v>507</v>
       </c>
       <c r="E134" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F134">
         <v>380702</v>
@@ -7255,7 +7257,7 @@
         <v>507</v>
       </c>
       <c r="E135" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F135">
         <v>1025036</v>
@@ -7285,7 +7287,7 @@
         <v>508</v>
       </c>
       <c r="E136" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F136">
         <v>380704</v>
@@ -7317,7 +7319,7 @@
         <v>509</v>
       </c>
       <c r="E137" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F137">
         <v>380611</v>
@@ -7349,7 +7351,7 @@
         <v>507</v>
       </c>
       <c r="E138" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F138">
         <v>417641</v>
@@ -7381,7 +7383,7 @@
         <v>509</v>
       </c>
       <c r="E139" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F139">
         <v>380612</v>
@@ -7413,7 +7415,7 @@
         <v>507</v>
       </c>
       <c r="E140" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F140">
         <v>380610</v>
@@ -7445,7 +7447,7 @@
         <v>507</v>
       </c>
       <c r="E141" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F141">
         <v>416138</v>
@@ -7477,7 +7479,7 @@
         <v>507</v>
       </c>
       <c r="E142" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F142">
         <v>416658</v>
@@ -7509,7 +7511,7 @@
         <v>508</v>
       </c>
       <c r="E143" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F143">
         <v>418420</v>
@@ -7541,7 +7543,7 @@
         <v>507</v>
       </c>
       <c r="E144" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F144">
         <v>380048</v>
@@ -7573,7 +7575,7 @@
         <v>507</v>
       </c>
       <c r="E145" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F145">
         <v>380049</v>
@@ -7605,7 +7607,7 @@
         <v>508</v>
       </c>
       <c r="E146" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F146">
         <v>380051</v>
@@ -7637,7 +7639,7 @@
         <v>508</v>
       </c>
       <c r="E147" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F147">
         <v>380052</v>
@@ -7669,7 +7671,7 @@
         <v>507</v>
       </c>
       <c r="E148" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F148">
         <v>380053</v>
@@ -7701,7 +7703,7 @@
         <v>509</v>
       </c>
       <c r="E149" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F149">
         <v>380054</v>
@@ -7733,7 +7735,7 @@
         <v>509</v>
       </c>
       <c r="E150" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F150">
         <v>413087</v>
@@ -7765,7 +7767,7 @@
         <v>509</v>
       </c>
       <c r="E151" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F151">
         <v>413088</v>
@@ -7797,7 +7799,7 @@
         <v>509</v>
       </c>
       <c r="E152" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F152">
         <v>380055</v>
@@ -7829,7 +7831,7 @@
         <v>507</v>
       </c>
       <c r="E153" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F153">
         <v>380992</v>
@@ -7861,7 +7863,7 @@
         <v>508</v>
       </c>
       <c r="E154" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F154">
         <v>383544</v>
@@ -7893,7 +7895,7 @@
         <v>508</v>
       </c>
       <c r="E155" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F155">
         <v>380993</v>
@@ -7925,7 +7927,7 @@
         <v>508</v>
       </c>
       <c r="E156" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F156">
         <v>381023</v>
@@ -7957,7 +7959,7 @@
         <v>508</v>
       </c>
       <c r="E157" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F157">
         <v>381024</v>
@@ -7989,7 +7991,7 @@
         <v>507</v>
       </c>
       <c r="E158" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F158">
         <v>381020</v>
@@ -8021,7 +8023,7 @@
         <v>509</v>
       </c>
       <c r="E159" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F159">
         <v>395247</v>
@@ -8053,7 +8055,7 @@
         <v>509</v>
       </c>
       <c r="E160" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F160">
         <v>381028</v>
@@ -8085,7 +8087,7 @@
         <v>508</v>
       </c>
       <c r="E161" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F161">
         <v>382917</v>
@@ -8117,7 +8119,7 @@
         <v>509</v>
       </c>
       <c r="E162" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F162">
         <v>380528</v>
@@ -8149,7 +8151,7 @@
         <v>509</v>
       </c>
       <c r="E163" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F163">
         <v>380529</v>
@@ -8181,7 +8183,7 @@
         <v>509</v>
       </c>
       <c r="E164" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F164">
         <v>380530</v>
@@ -8213,7 +8215,7 @@
         <v>509</v>
       </c>
       <c r="E165" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F165">
         <v>385002</v>
@@ -8245,7 +8247,7 @@
         <v>509</v>
       </c>
       <c r="E166" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F166">
         <v>385001</v>
@@ -8277,7 +8279,7 @@
         <v>509</v>
       </c>
       <c r="E167" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F167">
         <v>380531</v>
@@ -8309,7 +8311,7 @@
         <v>509</v>
       </c>
       <c r="E168" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F168">
         <v>380532</v>
@@ -8341,7 +8343,7 @@
         <v>509</v>
       </c>
       <c r="E169" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F169">
         <v>380541</v>
@@ -8373,7 +8375,7 @@
         <v>507</v>
       </c>
       <c r="E170" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F170">
         <v>380546</v>
@@ -8405,7 +8407,7 @@
         <v>509</v>
       </c>
       <c r="E171" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F171">
         <v>380548</v>
@@ -8437,7 +8439,7 @@
         <v>509</v>
       </c>
       <c r="E172" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F172">
         <v>380551</v>
@@ -8469,7 +8471,7 @@
         <v>507</v>
       </c>
       <c r="E173" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F173">
         <v>1023581</v>
@@ -8499,7 +8501,7 @@
         <v>507</v>
       </c>
       <c r="E174" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F174">
         <v>1024993</v>
@@ -8529,7 +8531,7 @@
         <v>507</v>
       </c>
       <c r="E175" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F175">
         <v>419698</v>
@@ -8561,7 +8563,7 @@
         <v>507</v>
       </c>
       <c r="E176" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F176">
         <v>1025543</v>
@@ -8591,7 +8593,7 @@
         <v>507</v>
       </c>
       <c r="E177" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F177">
         <v>1025545</v>
@@ -8621,7 +8623,7 @@
         <v>507</v>
       </c>
       <c r="E178" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F178">
         <v>1025547</v>
@@ -8651,7 +8653,7 @@
         <v>507</v>
       </c>
       <c r="E179" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F179">
         <v>1025652</v>
@@ -8681,7 +8683,7 @@
         <v>509</v>
       </c>
       <c r="E180" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F180">
         <v>419712</v>
@@ -8713,7 +8715,7 @@
         <v>509</v>
       </c>
       <c r="E181" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F181">
         <v>404624</v>
@@ -8745,7 +8747,7 @@
         <v>509</v>
       </c>
       <c r="E182" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F182">
         <v>404630</v>
@@ -8777,7 +8779,7 @@
         <v>509</v>
       </c>
       <c r="E183" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F183">
         <v>404632</v>
@@ -8809,7 +8811,7 @@
         <v>509</v>
       </c>
       <c r="E184" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F184">
         <v>380614</v>
@@ -8841,7 +8843,7 @@
         <v>509</v>
       </c>
       <c r="E185" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F185">
         <v>380615</v>
@@ -8873,7 +8875,7 @@
         <v>509</v>
       </c>
       <c r="E186" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F186">
         <v>380616</v>
@@ -8905,7 +8907,7 @@
         <v>509</v>
       </c>
       <c r="E187" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F187">
         <v>380617</v>
@@ -8937,7 +8939,7 @@
         <v>509</v>
       </c>
       <c r="E188" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F188">
         <v>380618</v>
@@ -8969,7 +8971,7 @@
         <v>507</v>
       </c>
       <c r="E189" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F189">
         <v>381941</v>
@@ -9001,7 +9003,7 @@
         <v>507</v>
       </c>
       <c r="E190" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F190">
         <v>382434</v>
@@ -9033,7 +9035,7 @@
         <v>507</v>
       </c>
       <c r="E191" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F191" s="2">
         <v>380102</v>
@@ -9065,7 +9067,7 @@
         <v>509</v>
       </c>
       <c r="E192" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F192" s="3">
         <v>380104</v>
@@ -9097,7 +9099,7 @@
         <v>507</v>
       </c>
       <c r="E193" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F193" s="3">
         <v>380291</v>
@@ -9129,7 +9131,7 @@
         <v>507</v>
       </c>
       <c r="E194" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F194" s="2">
         <v>380534</v>
@@ -9161,7 +9163,7 @@
         <v>507</v>
       </c>
       <c r="E195" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F195" s="2">
         <v>380535</v>
@@ -9193,7 +9195,7 @@
         <v>507</v>
       </c>
       <c r="E196" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F196" s="2">
         <v>380536</v>
@@ -9225,7 +9227,7 @@
         <v>507</v>
       </c>
       <c r="E197" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F197" s="2">
         <v>380537</v>
@@ -9257,7 +9259,7 @@
         <v>507</v>
       </c>
       <c r="E198" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F198" s="2">
         <v>380538</v>
@@ -9289,7 +9291,7 @@
         <v>507</v>
       </c>
       <c r="E199" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F199" s="2">
         <v>380539</v>
@@ -9321,7 +9323,7 @@
         <v>507</v>
       </c>
       <c r="E200" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F200" s="2">
         <v>380540</v>
@@ -9353,7 +9355,7 @@
         <v>507</v>
       </c>
       <c r="E201" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F201" s="2">
         <v>380542</v>
@@ -9385,7 +9387,7 @@
         <v>507</v>
       </c>
       <c r="E202" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F202" s="2">
         <v>380543</v>
@@ -9417,7 +9419,7 @@
         <v>507</v>
       </c>
       <c r="E203" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F203" s="2">
         <v>380544</v>
@@ -9449,7 +9451,7 @@
         <v>507</v>
       </c>
       <c r="E204" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F204" s="2">
         <v>380545</v>
@@ -9481,7 +9483,7 @@
         <v>507</v>
       </c>
       <c r="E205" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F205" s="4">
         <v>380547</v>
@@ -9513,7 +9515,7 @@
         <v>507</v>
       </c>
       <c r="E206" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F206" s="2">
         <v>380549</v>
@@ -9545,7 +9547,7 @@
         <v>507</v>
       </c>
       <c r="E207" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F207" s="2">
         <v>380550</v>
@@ -9577,7 +9579,7 @@
         <v>509</v>
       </c>
       <c r="E208" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F208" s="3">
         <v>380552</v>
@@ -9609,7 +9611,7 @@
         <v>507</v>
       </c>
       <c r="E209" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F209" s="2">
         <v>380554</v>
@@ -9641,7 +9643,7 @@
         <v>507</v>
       </c>
       <c r="E210" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F210" s="2">
         <v>380555</v>
@@ -9673,7 +9675,7 @@
         <v>507</v>
       </c>
       <c r="E211" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F211" s="2">
         <v>380556</v>
@@ -9705,7 +9707,7 @@
         <v>508</v>
       </c>
       <c r="E212" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F212" s="3">
         <v>380643</v>
@@ -9737,7 +9739,7 @@
         <v>509</v>
       </c>
       <c r="E213" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F213" s="3">
         <v>382788</v>
@@ -9769,7 +9771,7 @@
         <v>507</v>
       </c>
       <c r="E214" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F214" s="2">
         <v>385000</v>
@@ -9801,7 +9803,7 @@
         <v>507</v>
       </c>
       <c r="E215" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F215" s="2">
         <v>385003</v>
@@ -9833,7 +9835,7 @@
         <v>507</v>
       </c>
       <c r="E216" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F216" s="2">
         <v>404551</v>
@@ -9865,7 +9867,7 @@
         <v>507</v>
       </c>
       <c r="E217" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F217" s="2">
         <v>404587</v>
@@ -9897,7 +9899,7 @@
         <v>507</v>
       </c>
       <c r="E218" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F218" s="2">
         <v>404588</v>
@@ -9929,7 +9931,7 @@
         <v>509</v>
       </c>
       <c r="E219" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F219" s="3">
         <v>416107</v>
@@ -9961,7 +9963,7 @@
         <v>507</v>
       </c>
       <c r="E220" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F220" s="2">
         <v>416110</v>
@@ -9993,7 +9995,7 @@
         <v>507</v>
       </c>
       <c r="E221" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F221" s="2">
         <v>417722</v>
@@ -10025,7 +10027,7 @@
         <v>507</v>
       </c>
       <c r="E222" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F222" s="3">
         <v>417867</v>
@@ -10057,7 +10059,7 @@
         <v>507</v>
       </c>
       <c r="E223" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F223" s="2">
         <v>418130</v>
@@ -10089,7 +10091,7 @@
         <v>507</v>
       </c>
       <c r="E224" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F224" s="2">
         <v>419631</v>
@@ -10121,7 +10123,7 @@
         <v>507</v>
       </c>
       <c r="E225" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F225" s="2">
         <v>420877</v>
@@ -10153,7 +10155,7 @@
         <v>507</v>
       </c>
       <c r="E226" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F226" s="2">
         <v>427142</v>
@@ -10185,7 +10187,7 @@
         <v>507</v>
       </c>
       <c r="E227" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F227" s="2">
         <v>427287</v>
@@ -10217,7 +10219,7 @@
         <v>507</v>
       </c>
       <c r="E228" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F228" s="2">
         <v>428071</v>
@@ -10249,7 +10251,7 @@
         <v>507</v>
       </c>
       <c r="E229" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F229" s="4">
         <v>428564</v>
@@ -10281,7 +10283,7 @@
         <v>509</v>
       </c>
       <c r="E230" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F230" s="3">
         <v>428568</v>
@@ -10313,7 +10315,7 @@
         <v>507</v>
       </c>
       <c r="E231" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F231" s="2">
         <v>430503</v>
@@ -10345,7 +10347,7 @@
         <v>507</v>
       </c>
       <c r="E232" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F232" s="3">
         <v>431229</v>
@@ -10377,7 +10379,7 @@
         <v>507</v>
       </c>
       <c r="E233" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F233" s="2">
         <v>432102</v>
@@ -10409,7 +10411,7 @@
         <v>509</v>
       </c>
       <c r="E234" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F234" s="3">
         <v>432194</v>
@@ -10441,7 +10443,7 @@
         <v>509</v>
       </c>
       <c r="E235" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F235" s="3">
         <v>432195</v>
@@ -10473,7 +10475,7 @@
         <v>507</v>
       </c>
       <c r="E236" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F236" s="4">
         <v>432368</v>
@@ -10505,7 +10507,7 @@
         <v>507</v>
       </c>
       <c r="E237" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F237" s="2">
         <v>1023421</v>
@@ -10535,7 +10537,7 @@
         <v>507</v>
       </c>
       <c r="E238" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F238" s="2">
         <v>1023422</v>
@@ -10565,7 +10567,7 @@
         <v>507</v>
       </c>
       <c r="E239" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F239" s="2">
         <v>1023625</v>
@@ -10595,7 +10597,7 @@
         <v>507</v>
       </c>
       <c r="E240" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F240" s="2">
         <v>1023666</v>
@@ -10625,7 +10627,7 @@
         <v>507</v>
       </c>
       <c r="E241" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F241" s="2">
         <v>1023692</v>
@@ -10655,7 +10657,7 @@
         <v>507</v>
       </c>
       <c r="E242" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F242" s="2">
         <v>1023759</v>
@@ -10685,7 +10687,7 @@
         <v>507</v>
       </c>
       <c r="E243" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F243" s="2">
         <v>1023768</v>
@@ -10715,7 +10717,7 @@
         <v>507</v>
       </c>
       <c r="E244" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F244" s="2">
         <v>1023769</v>
@@ -10745,7 +10747,7 @@
         <v>507</v>
       </c>
       <c r="E245" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F245" s="2">
         <v>1024353</v>
@@ -10775,7 +10777,7 @@
         <v>507</v>
       </c>
       <c r="E246" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F246" s="2">
         <v>1024454</v>
@@ -10805,7 +10807,7 @@
         <v>507</v>
       </c>
       <c r="E247" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F247" s="2">
         <v>1024552</v>
@@ -10835,7 +10837,7 @@
         <v>507</v>
       </c>
       <c r="E248" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F248" s="2">
         <v>1024731</v>
@@ -10865,7 +10867,7 @@
         <v>508</v>
       </c>
       <c r="E249" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F249" s="2">
         <v>1024853</v>
@@ -10895,7 +10897,7 @@
         <v>508</v>
       </c>
       <c r="E250" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F250" s="2">
         <v>1025024</v>
@@ -10925,7 +10927,7 @@
         <v>507</v>
       </c>
       <c r="E251" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F251" s="2">
         <v>1025027</v>
@@ -10955,7 +10957,7 @@
         <v>509</v>
       </c>
       <c r="E252" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F252" s="2">
         <v>1025365</v>
@@ -10985,7 +10987,7 @@
         <v>508</v>
       </c>
       <c r="E253" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F253" s="2">
         <v>1025423</v>
@@ -11002,7 +11004,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:K253">
+  <autoFilter ref="A1:M253"/>
+  <sortState ref="A2:N253">
     <sortCondition ref="I1"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>